<commit_message>
Fixed Crossword Puzzle Comp +$150 bug where only $100 would be awarded
</commit_message>
<xml_diff>
--- a/Monopoly/Monopoly3.7/chance_data.xlsx
+++ b/Monopoly/Monopoly3.7/chance_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlee/Documents/Python/Personal-Projects/Monopoly/Monopoly3.7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E947B22-793B-824E-9C6B-83ABD95FD564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEBE0D2-E4EC-4345-8FDC-EB3FBFBB7D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25180" windowHeight="15440" xr2:uid="{EC51091A-2009-A44D-8957-CFFA10B8AF29}"/>
   </bookViews>
@@ -468,7 +468,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -708,7 +708,7 @@
         <v>16</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>